<commit_message>
Small ghoul worm typos
</commit_message>
<xml_diff>
--- a/data/Orcus - Monsters.xlsx
+++ b/data/Orcus - Monsters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Obsidian\Tabletop games\d20 System or D&amp;D-esque\2021 Orcus - 4E clone\GitHub\orcus\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B18BAD2-D293-43C7-B311-BEC899E9A1D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE8619D3-F05D-49D7-998F-91864428B809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6043" uniqueCount="1708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6043" uniqueCount="1709">
   <si>
     <t>Chapter</t>
   </si>
@@ -5214,6 +5214,9 @@
   <si>
     <t xml:space="preserve">##### Special
 The mega-chariot gives no XP. The ostovite swarm must be defeated for the heroes to gain XP. </t>
+  </si>
+  <si>
+    <t>Must be grappling the target</t>
   </si>
 </sst>
 </file>
@@ -5554,10 +5557,10 @@
   <dimension ref="A1:EZ174"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="AZ137" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L41" sqref="L41"/>
+      <selection pane="bottomRight" activeCell="BI147" sqref="BI147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -32437,11 +32440,8 @@
       <c r="BD147" s="2" t="s">
         <v>996</v>
       </c>
-      <c r="BF147" s="2">
-        <v>9</v>
-      </c>
       <c r="BH147" s="4" t="s">
-        <v>1207</v>
+        <v>1708</v>
       </c>
       <c r="BI147" s="2" t="s">
         <v>1662</v>
@@ -32493,9 +32493,6 @@
       </c>
       <c r="CA147" s="2" t="s">
         <v>996</v>
-      </c>
-      <c r="CB147" s="2">
-        <v>9</v>
       </c>
       <c r="CC147" s="2" t="s">
         <v>996</v>

</xml_diff>